<commit_message>
fix the test by adding back working.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/config/config.xlsx
+++ b/src/test/resources/config/config.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d065350/Documents/workspace/cloud-realspend-expenses-uploader/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d065350/Documents/workspace/cloud-realspend-expenses-uploader/src/test/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Center Actuals" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
   <si>
     <t>User</t>
   </si>
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,51 +451,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5">
         <v>1104340</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1104340</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1104341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1104342</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1104340</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -504,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,40 +500,12 @@
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3">
-        <v>4000000</v>
+        <v>10000000</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>5000000</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -580,10 +516,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,49 +551,15 @@
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5">
         <v>1104340</v>
       </c>
       <c r="D2" s="3">
-        <v>4000000</v>
+        <v>12000</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1104341</v>
-      </c>
-      <c r="D3" s="3">
-        <v>5000000</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1104342</v>
-      </c>
-      <c r="D4" s="3">
-        <v>10000000</v>
-      </c>
-      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -757,7 +659,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added config example file
</commit_message>
<xml_diff>
--- a/src/test/resources/config/config.xlsx
+++ b/src/test/resources/config/config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Center Actuals" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="13">
   <si>
     <t>User</t>
   </si>
@@ -39,15 +39,6 @@
     <t>Cost Center</t>
   </si>
   <si>
-    <t>S12345678</t>
-  </si>
-  <si>
-    <t>S12345679</t>
-  </si>
-  <si>
-    <t>S12345670</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
   </si>
   <si>
     <t>Product B</t>
-  </si>
-  <si>
-    <t>Product C</t>
   </si>
   <si>
     <t>p1942234997</t>
@@ -88,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,11 +96,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,13 +128,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,9 +433,9 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="5">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4">
         <v>1104340</v>
       </c>
     </row>
@@ -483,16 +465,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -500,13 +482,13 @@
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3">
         <v>10000000</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -518,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,7 +513,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -540,10 +522,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -551,16 +533,16 @@
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4">
         <v>1104340</v>
       </c>
       <c r="D2" s="3">
         <v>12000</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -570,10 +552,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,19 +565,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -603,16 +585,16 @@
         <v>2015</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C2" s="3">
-        <v>6414000000</v>
+        <v>6478000000</v>
       </c>
       <c r="D2" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -620,16 +602,16 @@
         <v>2015</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3">
-        <v>6478000000</v>
+        <v>3273500000</v>
       </c>
       <c r="D3" s="3">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -637,17 +619,156 @@
         <v>2015</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3">
-        <v>6490512000</v>
+        <v>6410000100</v>
       </c>
       <c r="D4" s="3">
         <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6412000000</v>
+      </c>
+      <c r="D5" s="3">
+        <v>299</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>6412000200</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6412600000</v>
+      </c>
+      <c r="D7" s="3">
+        <v>500</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>6413000000</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>6413000100</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3">
+        <v>6414000000</v>
+      </c>
+      <c r="D10" s="3">
+        <v>300</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6414900000</v>
+      </c>
+      <c r="D11" s="3">
+        <v>350</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <v>6416500000</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -656,10 +777,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G15"/>
+  <dimension ref="B1:G3"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,22 +790,22 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
@@ -692,19 +813,19 @@
         <v>2015</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -712,215 +833,19 @@
         <v>2015</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3">
-        <v>300</v>
+        <v>800</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="3">
-        <v>5000</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3">
-        <v>100</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="3">
-        <v>900</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="3">
-        <v>700</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="3">
-        <v>300</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="3">
-        <v>12000</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="3">
-        <v>2015</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1289</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>